<commit_message>
Improve command line messages adni-to-bids
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications_adni.xlsx
+++ b/clinica/iotools/data/clinical_specifications_adni.xlsx
@@ -2881,7 +2881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -8455,7 +8455,7 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adni cdr clinical data
</commit_message>
<xml_diff>
--- a/clinica/iotools/data/clinical_specifications_adni.xlsx
+++ b/clinica/iotools/data/clinical_specifications_adni.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabrina.fontanella/PyCharmPrograms/clinica/clinica/iotools/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simona.bottani/clinica/clinica/iotools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-62460" yWindow="-4540" windowWidth="28700" windowHeight="14700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="167">
   <si>
     <t>Field</t>
   </si>
@@ -541,6 +541,18 @@
   </si>
   <si>
     <t>MMS</t>
+  </si>
+  <si>
+    <t>CDGLOBAL</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>cdr_global</t>
+  </si>
+  <si>
+    <t>CDR.CSV</t>
   </si>
 </sst>
 </file>
@@ -812,80 +824,80 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="75">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2613,6 +2625,174 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8452,10 +8632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8623,389 +8803,403 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
-        <v>25</v>
+        <v>163</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>162</v>
+        <v>165</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>102</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>26</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>102</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>102</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>102</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>102</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
-        <v>34</v>
-      </c>
       <c r="B20" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>102</v>
       </c>
       <c r="D20" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-    </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>129</v>
-      </c>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D34" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D48" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D70" s="16"/>
-    </row>
     <row r="71" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="25"/>
       <c r="D71" s="16"/>
     </row>
     <row r="72" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="25"/>
       <c r="D72" s="16"/>
     </row>
     <row r="73" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="25"/>
       <c r="D73" s="16"/>
+    </row>
+    <row r="74" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="25"/>
+      <c r="D74" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>